<commit_message>
Icono y titulo de pestaña del sistema modificado
</commit_message>
<xml_diff>
--- a/public/week_data.xlsx
+++ b/public/week_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
   <si>
     <t>USUARIO ORLANDO BEJARANO FERNANDEZ</t>
   </si>
@@ -77,15 +77,15 @@
     <t>2022-04-27</t>
   </si>
   <si>
+    <t>PAOLA RAQUEL PIMENTEL ROMERO</t>
+  </si>
+  <si>
+    <t>2022-05-03</t>
+  </si>
+  <si>
     <t>SERGIO ROCHA ALARCON</t>
   </si>
   <si>
-    <t>2022-05-03</t>
-  </si>
-  <si>
-    <t>PAOLA RAQUEL PIMENTEL ROMERO</t>
-  </si>
-  <si>
     <t>2022-05-04</t>
   </si>
   <si>
@@ -161,21 +161,21 @@
     <t>2022-07-26</t>
   </si>
   <si>
+    <t>2022-07-30</t>
+  </si>
+  <si>
     <t>POLONIA JEREZ RUEDA</t>
   </si>
   <si>
-    <t>2022-07-30</t>
-  </si>
-  <si>
     <t>2022-08-01</t>
   </si>
   <si>
+    <t>JHOVANA ANGELICA RUEDA MARTINEZ</t>
+  </si>
+  <si>
     <t>2022-08-06</t>
   </si>
   <si>
-    <t>JHOVANA ANGELICA RUEDA MARTINEZ</t>
-  </si>
-  <si>
     <t>2022-08-08</t>
   </si>
   <si>
@@ -359,10 +359,76 @@
     <t>2022-12-22</t>
   </si>
   <si>
+    <t>MARCO ANTONIO COLODRO</t>
+  </si>
+  <si>
     <t>LISELDA MILENIA ROMERO ALARCON</t>
   </si>
   <si>
-    <t>MARCO ANTONIO COLODRO</t>
+    <t>2022-12-26</t>
+  </si>
+  <si>
+    <t>VICTOR EMERSON CARTAGENA CASTRO</t>
+  </si>
+  <si>
+    <t>2022-12-27</t>
+  </si>
+  <si>
+    <t>2023-01-02</t>
+  </si>
+  <si>
+    <t>2023-01-04</t>
+  </si>
+  <si>
+    <t>2023-01-05</t>
+  </si>
+  <si>
+    <t>2023-01-09</t>
+  </si>
+  <si>
+    <t>2023-01-11</t>
+  </si>
+  <si>
+    <t>2023-01-16</t>
+  </si>
+  <si>
+    <t>2023-01-18</t>
+  </si>
+  <si>
+    <t>2023-01-19</t>
+  </si>
+  <si>
+    <t>2023-01-23</t>
+  </si>
+  <si>
+    <t>2023-01-25</t>
+  </si>
+  <si>
+    <t>2023-01-30</t>
+  </si>
+  <si>
+    <t>2023-02-01</t>
+  </si>
+  <si>
+    <t>2023-02-02</t>
+  </si>
+  <si>
+    <t>2023-02-06</t>
+  </si>
+  <si>
+    <t>2023-02-15</t>
+  </si>
+  <si>
+    <t>2023-02-25</t>
+  </si>
+  <si>
+    <t>2023-03-01</t>
+  </si>
+  <si>
+    <t>2023-03-15</t>
+  </si>
+  <si>
+    <t>2023-03-29</t>
   </si>
   <si>
     <t xml:space="preserve">FILTRO: </t>
@@ -373,7 +439,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -408,15 +474,6 @@
       <u val="none"/>
       <sz val="11"/>
       <color rgb="FF800000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FF008000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -454,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -474,9 +531,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -813,10 +867,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N117"/>
+  <dimension ref="A1:N143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B117" sqref="B117"/>
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -853,14 +907,12 @@
         <v>7</v>
       </c>
       <c r="K6" s="4">
-        <v>76343.96</v>
+        <v>121738.76</v>
       </c>
       <c r="L6" s="4"/>
-      <c r="M6" s="4">
-        <v>8952.1</v>
-      </c>
+      <c r="M6" s="4"/>
       <c r="N6" s="4">
-        <v>85296.06</v>
+        <v>121738.76</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1015,7 +1067,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="4">
-        <v>7162716</v>
+        <v>10651336</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>20</v>
@@ -1033,7 +1085,7 @@
         <v>7</v>
       </c>
       <c r="K13" s="4">
-        <v>1235.0</v>
+        <v>665.0</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>21</v>
@@ -1045,7 +1097,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="4">
-        <v>10651336</v>
+        <v>7162716</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>22</v>
@@ -1063,7 +1115,7 @@
         <v>7</v>
       </c>
       <c r="K14" s="4">
-        <v>665.0</v>
+        <v>1235.0</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>21</v>
@@ -1138,7 +1190,7 @@
         <v>10651336</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1195,10 +1247,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="4">
-        <v>5784526</v>
+        <v>7162716</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1213,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="K19" s="4">
-        <v>498.1</v>
+        <v>1235.0</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>28</v>
@@ -1225,10 +1277,10 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="4">
-        <v>7162716</v>
+        <v>5784526</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1243,7 +1295,7 @@
         <v>7</v>
       </c>
       <c r="K20" s="4">
-        <v>1235.0</v>
+        <v>498.1</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>28</v>
@@ -1288,7 +1340,7 @@
         <v>10651336</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1378,7 +1430,7 @@
         <v>7162716</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1468,7 +1520,7 @@
         <v>10651336</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1528,7 +1580,7 @@
         <v>7162716</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1588,7 +1640,7 @@
         <v>10651336</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -1648,7 +1700,7 @@
         <v>7162716</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1708,7 +1760,7 @@
         <v>10651336</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1768,7 +1820,7 @@
         <v>7162716</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -1825,10 +1877,10 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="4">
-        <v>5787275</v>
+        <v>10651336</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -1843,10 +1895,10 @@
         <v>7</v>
       </c>
       <c r="K40" s="4">
-        <v>210.6</v>
+        <v>665.0</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="6" t="s">
@@ -1855,10 +1907,10 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="4">
-        <v>10651336</v>
+        <v>5787275</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -1873,10 +1925,10 @@
         <v>7</v>
       </c>
       <c r="K41" s="4">
-        <v>665.0</v>
+        <v>210.6</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M41" s="4"/>
       <c r="N41" s="6" t="s">
@@ -1888,7 +1940,7 @@
         <v>7162716</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -1915,10 +1967,10 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="4">
-        <v>5787275</v>
+        <v>7118244</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -1933,10 +1985,10 @@
         <v>7</v>
       </c>
       <c r="K43" s="4">
-        <v>1010.6</v>
+        <v>1980.0</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M43" s="4"/>
       <c r="N43" s="6" t="s">
@@ -1945,10 +1997,10 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" s="4">
-        <v>7118244</v>
+        <v>5787275</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -1963,10 +2015,10 @@
         <v>7</v>
       </c>
       <c r="K44" s="4">
-        <v>1980.0</v>
+        <v>1010.6</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M44" s="4"/>
       <c r="N44" s="6" t="s">
@@ -2008,7 +2060,7 @@
         <v>5787275</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -2035,7 +2087,7 @@
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="4">
-        <v>7162716</v>
+        <v>10651336</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>20</v>
@@ -2053,7 +2105,7 @@
         <v>7</v>
       </c>
       <c r="K47" s="4">
-        <v>1235.0</v>
+        <v>665.0</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>55</v>
@@ -2065,7 +2117,7 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="4">
-        <v>10651336</v>
+        <v>7162716</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>22</v>
@@ -2083,7 +2135,7 @@
         <v>7</v>
       </c>
       <c r="K48" s="4">
-        <v>665.0</v>
+        <v>1235.0</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>55</v>
@@ -2128,7 +2180,7 @@
         <v>5787275</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -2158,7 +2210,7 @@
         <v>7118244</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
@@ -2188,7 +2240,7 @@
         <v>5787275</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -2218,7 +2270,7 @@
         <v>7162716</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -2245,10 +2297,10 @@
     </row>
     <row r="54" spans="1:14">
       <c r="A54" s="4">
-        <v>5787275</v>
+        <v>7143371</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -2263,7 +2315,7 @@
         <v>7</v>
       </c>
       <c r="K54" s="4">
-        <v>1010.6</v>
+        <v>287.47</v>
       </c>
       <c r="L54" s="5" t="s">
         <v>62</v>
@@ -2275,10 +2327,10 @@
     </row>
     <row r="55" spans="1:14">
       <c r="A55" s="4">
-        <v>7143371</v>
+        <v>5787275</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -2293,7 +2345,7 @@
         <v>7</v>
       </c>
       <c r="K55" s="4">
-        <v>287.47</v>
+        <v>1010.6</v>
       </c>
       <c r="L55" s="5" t="s">
         <v>62</v>
@@ -2308,7 +2360,7 @@
         <v>5787275</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -2368,7 +2420,7 @@
         <v>7162716</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -2398,7 +2450,7 @@
         <v>5787275</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -2458,7 +2510,7 @@
         <v>5787275</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -2548,7 +2600,7 @@
         <v>5787275</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -2698,7 +2750,7 @@
         <v>5787275</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
@@ -2818,7 +2870,7 @@
         <v>5787275</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -2905,10 +2957,10 @@
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="4">
-        <v>1899092</v>
+        <v>7143371</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -2923,7 +2975,7 @@
         <v>7</v>
       </c>
       <c r="K76" s="4">
-        <v>770.0</v>
+        <v>287.47</v>
       </c>
       <c r="L76" s="5" t="s">
         <v>85</v>
@@ -2935,10 +2987,10 @@
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="4">
-        <v>7143371</v>
+        <v>1899092</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -2953,7 +3005,7 @@
         <v>7</v>
       </c>
       <c r="K77" s="4">
-        <v>287.47</v>
+        <v>770.0</v>
       </c>
       <c r="L77" s="5" t="s">
         <v>85</v>
@@ -2998,7 +3050,7 @@
         <v>5787275</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -3115,10 +3167,10 @@
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="4">
-        <v>5787275</v>
+        <v>5684823</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -3133,7 +3185,7 @@
         <v>7</v>
       </c>
       <c r="K83" s="4">
-        <v>1010.6</v>
+        <v>665.0</v>
       </c>
       <c r="L83" s="5" t="s">
         <v>90</v>
@@ -3145,10 +3197,10 @@
     </row>
     <row r="84" spans="1:14">
       <c r="A84" s="4">
-        <v>5684823</v>
+        <v>5787275</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
@@ -3163,7 +3215,7 @@
         <v>7</v>
       </c>
       <c r="K84" s="4">
-        <v>665.0</v>
+        <v>1010.6</v>
       </c>
       <c r="L84" s="5" t="s">
         <v>90</v>
@@ -3175,10 +3227,10 @@
     </row>
     <row r="85" spans="1:14">
       <c r="A85" s="4">
-        <v>1899092</v>
+        <v>7259089</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
@@ -3193,7 +3245,7 @@
         <v>7</v>
       </c>
       <c r="K85" s="4">
-        <v>770.0</v>
+        <v>818.38</v>
       </c>
       <c r="L85" s="5" t="s">
         <v>91</v>
@@ -3205,10 +3257,10 @@
     </row>
     <row r="86" spans="1:14">
       <c r="A86" s="4">
-        <v>7259089</v>
+        <v>1899092</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
@@ -3223,7 +3275,7 @@
         <v>7</v>
       </c>
       <c r="K86" s="4">
-        <v>818.38</v>
+        <v>770.0</v>
       </c>
       <c r="L86" s="5" t="s">
         <v>91</v>
@@ -3298,7 +3350,7 @@
         <v>5787275</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
@@ -3388,7 +3440,7 @@
         <v>5787275</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
@@ -3415,10 +3467,10 @@
     </row>
     <row r="93" spans="1:14">
       <c r="A93" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
@@ -3433,7 +3485,7 @@
         <v>7</v>
       </c>
       <c r="K93" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L93" s="5" t="s">
         <v>97</v>
@@ -3445,10 +3497,10 @@
     </row>
     <row r="94" spans="1:14">
       <c r="A94" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
@@ -3463,7 +3515,7 @@
         <v>7</v>
       </c>
       <c r="K94" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L94" s="5" t="s">
         <v>97</v>
@@ -3475,10 +3527,10 @@
     </row>
     <row r="95" spans="1:14">
       <c r="A95" s="4">
-        <v>5684823</v>
+        <v>1899092</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
@@ -3493,7 +3545,7 @@
         <v>7</v>
       </c>
       <c r="K95" s="4">
-        <v>665.0</v>
+        <v>770.0</v>
       </c>
       <c r="L95" s="5" t="s">
         <v>98</v>
@@ -3505,10 +3557,10 @@
     </row>
     <row r="96" spans="1:14">
       <c r="A96" s="4">
-        <v>1899092</v>
+        <v>5684823</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
@@ -3523,7 +3575,7 @@
         <v>7</v>
       </c>
       <c r="K96" s="4">
-        <v>770.0</v>
+        <v>665.0</v>
       </c>
       <c r="L96" s="5" t="s">
         <v>98</v>
@@ -3568,7 +3620,7 @@
         <v>5787275</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
@@ -3658,7 +3710,7 @@
         <v>5787275</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
@@ -3715,10 +3767,10 @@
     </row>
     <row r="103" spans="1:14">
       <c r="A103" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
@@ -3733,7 +3785,7 @@
         <v>7</v>
       </c>
       <c r="K103" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L103" s="5" t="s">
         <v>103</v>
@@ -3745,10 +3797,10 @@
     </row>
     <row r="104" spans="1:14">
       <c r="A104" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
@@ -3763,7 +3815,7 @@
         <v>7</v>
       </c>
       <c r="K104" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L104" s="5" t="s">
         <v>103</v>
@@ -3778,7 +3830,7 @@
         <v>5787275</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
@@ -3979,8 +4031,8 @@
         <v>109</v>
       </c>
       <c r="M111" s="4"/>
-      <c r="N111" s="7" t="s">
-        <v>5</v>
+      <c r="N111" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:14">
@@ -4009,8 +4061,8 @@
         <v>111</v>
       </c>
       <c r="M112" s="4"/>
-      <c r="N112" s="7" t="s">
-        <v>5</v>
+      <c r="N112" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:14">
@@ -4039,13 +4091,13 @@
         <v>113</v>
       </c>
       <c r="M113" s="4"/>
-      <c r="N113" s="7" t="s">
-        <v>5</v>
+      <c r="N113" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="4">
-        <v>7247912</v>
+        <v>7190526</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>114</v>
@@ -4063,19 +4115,19 @@
         <v>7</v>
       </c>
       <c r="K114" s="4">
-        <v>8000.0</v>
+        <v>57.0</v>
       </c>
       <c r="L114" s="5" t="s">
         <v>113</v>
       </c>
       <c r="M114" s="4"/>
-      <c r="N114" s="7" t="s">
-        <v>5</v>
+      <c r="N114" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="4">
-        <v>7190526</v>
+        <v>7247912</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>115</v>
@@ -4093,21 +4145,801 @@
         <v>7</v>
       </c>
       <c r="K115" s="4">
-        <v>57.0</v>
+        <v>8000.0</v>
       </c>
       <c r="L115" s="5" t="s">
         <v>113</v>
       </c>
       <c r="M115" s="4"/>
-      <c r="N115" s="7" t="s">
-        <v>5</v>
+      <c r="N115" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14">
+      <c r="A116" s="4">
+        <v>7254095</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="4"/>
+      <c r="J116" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K116" s="4">
+        <v>185.1</v>
+      </c>
+      <c r="L116" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M116" s="4"/>
+      <c r="N116" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:14">
-      <c r="A117" t="s">
+      <c r="A117" s="4">
+        <v>5021478</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G117" s="4"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="4"/>
+      <c r="J117" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K117" s="4">
+        <v>1480.0</v>
+      </c>
+      <c r="L117" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B117" t="s">
+      <c r="M117" s="4"/>
+      <c r="N117" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14">
+      <c r="A118" s="4">
+        <v>7103441</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="4"/>
+      <c r="J118" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K118" s="4">
+        <v>1480.0</v>
+      </c>
+      <c r="L118" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="M118" s="4"/>
+      <c r="N118" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14">
+      <c r="A119" s="4">
+        <v>7254095</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G119" s="4"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="4"/>
+      <c r="J119" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K119" s="4">
+        <v>185.1</v>
+      </c>
+      <c r="L119" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M119" s="4"/>
+      <c r="N119" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14">
+      <c r="A120" s="4">
+        <v>5032867</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="4"/>
+      <c r="J120" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K120" s="4">
+        <v>390.0</v>
+      </c>
+      <c r="L120" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="M120" s="4"/>
+      <c r="N120" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14">
+      <c r="A121" s="4">
+        <v>7247912</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G121" s="4"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="4"/>
+      <c r="J121" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K121" s="4">
+        <v>8000.0</v>
+      </c>
+      <c r="L121" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="M121" s="4"/>
+      <c r="N121" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14">
+      <c r="A122" s="4">
+        <v>5797560</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="4"/>
+      <c r="J122" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K122" s="4">
+        <v>320.0</v>
+      </c>
+      <c r="L122" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="M122" s="4"/>
+      <c r="N122" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14">
+      <c r="A123" s="4">
+        <v>7190526</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G123" s="4"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="4"/>
+      <c r="J123" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K123" s="4">
+        <v>57.0</v>
+      </c>
+      <c r="L123" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="M123" s="4"/>
+      <c r="N123" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14">
+      <c r="A124" s="4">
+        <v>7254095</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G124" s="4"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="4"/>
+      <c r="J124" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K124" s="4">
+        <v>185.1</v>
+      </c>
+      <c r="L124" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="M124" s="4"/>
+      <c r="N124" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14">
+      <c r="A125" s="4">
+        <v>7103441</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="4"/>
+      <c r="J125" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K125" s="4">
+        <v>1480.0</v>
+      </c>
+      <c r="L125" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="M125" s="4"/>
+      <c r="N125" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14">
+      <c r="A126" s="4">
+        <v>7254095</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G126" s="4"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="4"/>
+      <c r="J126" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K126" s="4">
+        <v>185.1</v>
+      </c>
+      <c r="L126" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M126" s="4"/>
+      <c r="N126" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14">
+      <c r="A127" s="4">
+        <v>5032867</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G127" s="4"/>
+      <c r="H127" s="4"/>
+      <c r="I127" s="4"/>
+      <c r="J127" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K127" s="4">
+        <v>390.0</v>
+      </c>
+      <c r="L127" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="M127" s="4"/>
+      <c r="N127" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14">
+      <c r="A128" s="4">
+        <v>5797560</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G128" s="4"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="4"/>
+      <c r="J128" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K128" s="4">
+        <v>320.0</v>
+      </c>
+      <c r="L128" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="M128" s="4"/>
+      <c r="N128" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14">
+      <c r="A129" s="4">
+        <v>7247912</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G129" s="4"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="4"/>
+      <c r="J129" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K129" s="4">
+        <v>8000.0</v>
+      </c>
+      <c r="L129" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="M129" s="4"/>
+      <c r="N129" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14">
+      <c r="A130" s="4">
+        <v>7254095</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C130" s="4"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G130" s="4"/>
+      <c r="H130" s="4"/>
+      <c r="I130" s="4"/>
+      <c r="J130" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K130" s="4">
+        <v>185.1</v>
+      </c>
+      <c r="L130" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="M130" s="4"/>
+      <c r="N130" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14">
+      <c r="A131" s="4">
+        <v>5021478</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C131" s="4"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G131" s="4"/>
+      <c r="H131" s="4"/>
+      <c r="I131" s="4"/>
+      <c r="J131" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K131" s="4">
+        <v>1480.0</v>
+      </c>
+      <c r="L131" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="M131" s="4"/>
+      <c r="N131" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14">
+      <c r="A132" s="4">
+        <v>7254095</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G132" s="4"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="4"/>
+      <c r="J132" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K132" s="4">
+        <v>185.1</v>
+      </c>
+      <c r="L132" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="M132" s="4"/>
+      <c r="N132" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14">
+      <c r="A133" s="4">
+        <v>5032867</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C133" s="4"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="4"/>
+      <c r="F133" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G133" s="4"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="4"/>
+      <c r="J133" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K133" s="4">
+        <v>390.0</v>
+      </c>
+      <c r="L133" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="M133" s="4"/>
+      <c r="N133" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14">
+      <c r="A134" s="4">
+        <v>7247912</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C134" s="4"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G134" s="4"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="4"/>
+      <c r="J134" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K134" s="4">
+        <v>8000.0</v>
+      </c>
+      <c r="L134" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="M134" s="4"/>
+      <c r="N134" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14">
+      <c r="A135" s="4">
+        <v>5797560</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C135" s="4"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G135" s="4"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="4"/>
+      <c r="J135" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K135" s="4">
+        <v>320.0</v>
+      </c>
+      <c r="L135" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="M135" s="4"/>
+      <c r="N135" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14">
+      <c r="A136" s="4">
+        <v>7254095</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C136" s="4"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G136" s="4"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="4"/>
+      <c r="J136" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K136" s="4">
+        <v>185.1</v>
+      </c>
+      <c r="L136" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="M136" s="4"/>
+      <c r="N136" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14">
+      <c r="A137" s="4">
+        <v>5032867</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C137" s="4"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G137" s="4"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="4"/>
+      <c r="J137" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K137" s="4">
+        <v>390.0</v>
+      </c>
+      <c r="L137" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="M137" s="4"/>
+      <c r="N137" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14">
+      <c r="A138" s="4">
+        <v>5021478</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C138" s="4"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="4"/>
+      <c r="F138" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G138" s="4"/>
+      <c r="H138" s="4"/>
+      <c r="I138" s="4"/>
+      <c r="J138" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K138" s="4">
+        <v>1480.0</v>
+      </c>
+      <c r="L138" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="M138" s="4"/>
+      <c r="N138" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14">
+      <c r="A139" s="4">
+        <v>5032867</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C139" s="4"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="4"/>
+      <c r="F139" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G139" s="4"/>
+      <c r="H139" s="4"/>
+      <c r="I139" s="4"/>
+      <c r="J139" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K139" s="4">
+        <v>390.0</v>
+      </c>
+      <c r="L139" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="M139" s="4"/>
+      <c r="N139" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14">
+      <c r="A140" s="4">
+        <v>5032867</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C140" s="4"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="4"/>
+      <c r="F140" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G140" s="4"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+      <c r="J140" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K140" s="4">
+        <v>390.0</v>
+      </c>
+      <c r="L140" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="M140" s="4"/>
+      <c r="N140" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14">
+      <c r="A141" s="4">
+        <v>5032867</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C141" s="4"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G141" s="4"/>
+      <c r="H141" s="4"/>
+      <c r="I141" s="4"/>
+      <c r="J141" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K141" s="4">
+        <v>390.0</v>
+      </c>
+      <c r="L141" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="M141" s="4"/>
+      <c r="N141" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14">
+      <c r="A143" t="s">
+        <v>138</v>
+      </c>
+      <c r="B143" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4440,13 +5272,91 @@
     <mergeCell ref="B115:E115"/>
     <mergeCell ref="F115:I115"/>
     <mergeCell ref="L115:M115"/>
-    <mergeCell ref="B117:N117"/>
+    <mergeCell ref="B116:E116"/>
+    <mergeCell ref="F116:I116"/>
+    <mergeCell ref="L116:M116"/>
+    <mergeCell ref="B117:E117"/>
+    <mergeCell ref="F117:I117"/>
+    <mergeCell ref="L117:M117"/>
+    <mergeCell ref="B118:E118"/>
+    <mergeCell ref="F118:I118"/>
+    <mergeCell ref="L118:M118"/>
+    <mergeCell ref="B119:E119"/>
+    <mergeCell ref="F119:I119"/>
+    <mergeCell ref="L119:M119"/>
+    <mergeCell ref="B120:E120"/>
+    <mergeCell ref="F120:I120"/>
+    <mergeCell ref="L120:M120"/>
+    <mergeCell ref="B121:E121"/>
+    <mergeCell ref="F121:I121"/>
+    <mergeCell ref="L121:M121"/>
+    <mergeCell ref="B122:E122"/>
+    <mergeCell ref="F122:I122"/>
+    <mergeCell ref="L122:M122"/>
+    <mergeCell ref="B123:E123"/>
+    <mergeCell ref="F123:I123"/>
+    <mergeCell ref="L123:M123"/>
+    <mergeCell ref="B124:E124"/>
+    <mergeCell ref="F124:I124"/>
+    <mergeCell ref="L124:M124"/>
+    <mergeCell ref="B125:E125"/>
+    <mergeCell ref="F125:I125"/>
+    <mergeCell ref="L125:M125"/>
+    <mergeCell ref="B126:E126"/>
+    <mergeCell ref="F126:I126"/>
+    <mergeCell ref="L126:M126"/>
+    <mergeCell ref="B127:E127"/>
+    <mergeCell ref="F127:I127"/>
+    <mergeCell ref="L127:M127"/>
+    <mergeCell ref="B128:E128"/>
+    <mergeCell ref="F128:I128"/>
+    <mergeCell ref="L128:M128"/>
+    <mergeCell ref="B129:E129"/>
+    <mergeCell ref="F129:I129"/>
+    <mergeCell ref="L129:M129"/>
+    <mergeCell ref="B130:E130"/>
+    <mergeCell ref="F130:I130"/>
+    <mergeCell ref="L130:M130"/>
+    <mergeCell ref="B131:E131"/>
+    <mergeCell ref="F131:I131"/>
+    <mergeCell ref="L131:M131"/>
+    <mergeCell ref="B132:E132"/>
+    <mergeCell ref="F132:I132"/>
+    <mergeCell ref="L132:M132"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="F133:I133"/>
+    <mergeCell ref="L133:M133"/>
+    <mergeCell ref="B134:E134"/>
+    <mergeCell ref="F134:I134"/>
+    <mergeCell ref="L134:M134"/>
+    <mergeCell ref="B135:E135"/>
+    <mergeCell ref="F135:I135"/>
+    <mergeCell ref="L135:M135"/>
+    <mergeCell ref="B136:E136"/>
+    <mergeCell ref="F136:I136"/>
+    <mergeCell ref="L136:M136"/>
+    <mergeCell ref="B137:E137"/>
+    <mergeCell ref="F137:I137"/>
+    <mergeCell ref="L137:M137"/>
+    <mergeCell ref="B138:E138"/>
+    <mergeCell ref="F138:I138"/>
+    <mergeCell ref="L138:M138"/>
+    <mergeCell ref="B139:E139"/>
+    <mergeCell ref="F139:I139"/>
+    <mergeCell ref="L139:M139"/>
+    <mergeCell ref="B140:E140"/>
+    <mergeCell ref="F140:I140"/>
+    <mergeCell ref="L140:M140"/>
+    <mergeCell ref="B141:E141"/>
+    <mergeCell ref="F141:I141"/>
+    <mergeCell ref="L141:M141"/>
+    <mergeCell ref="B143:N143"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="73" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader>&amp;L2022-12-15 10:47:17&amp;C&amp;HECOMSOFT&amp;RDR. ORLANDO BEJARANO FERNANDEZ</oddHeader>
+    <oddHeader>&amp;L2024-02-15 07:40:52&amp;C&amp;HECOMSOFT&amp;RDR. ORLANDO BEJARANO FERNANDEZ</oddHeader>
     <oddFooter>&amp;RPage &amp;P of &amp;N</oddFooter>
     <evenHeader/>
     <evenFooter/>

</xml_diff>

<commit_message>
Ultimo cambio despues de publicarlo en el dominio
</commit_message>
<xml_diff>
--- a/public/week_data.xlsx
+++ b/public/week_data.xlsx
@@ -170,12 +170,12 @@
     <t>2022-08-01</t>
   </si>
   <si>
+    <t>2022-08-06</t>
+  </si>
+  <si>
     <t>JHOVANA ANGELICA RUEDA MARTINEZ</t>
   </si>
   <si>
-    <t>2022-08-06</t>
-  </si>
-  <si>
     <t>2022-08-08</t>
   </si>
   <si>
@@ -239,10 +239,10 @@
     <t>2022-09-29</t>
   </si>
   <si>
+    <t>TATIANA TRUJILLO VASQUEZ</t>
+  </si>
+  <si>
     <t>2022-10-01</t>
-  </si>
-  <si>
-    <t>TATIANA TRUJILLO VASQUEZ</t>
   </si>
   <si>
     <t>2022-10-03</t>
@@ -1367,10 +1367,10 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="4">
-        <v>7217197</v>
+        <v>5784526</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1385,7 +1385,7 @@
         <v>7</v>
       </c>
       <c r="K23" s="4">
-        <v>950.0</v>
+        <v>498.1</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>31</v>
@@ -1397,10 +1397,10 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="4">
-        <v>5784526</v>
+        <v>7217197</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1415,7 +1415,7 @@
         <v>7</v>
       </c>
       <c r="K24" s="4">
-        <v>498.1</v>
+        <v>950.0</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>31</v>
@@ -1967,10 +1967,10 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="4">
-        <v>7118244</v>
+        <v>5787275</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -1985,10 +1985,10 @@
         <v>7</v>
       </c>
       <c r="K43" s="4">
-        <v>1980.0</v>
+        <v>1010.6</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M43" s="4"/>
       <c r="N43" s="6" t="s">
@@ -1997,10 +1997,10 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" s="4">
-        <v>5787275</v>
+        <v>7118244</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -2015,10 +2015,10 @@
         <v>7</v>
       </c>
       <c r="K44" s="4">
-        <v>1010.6</v>
+        <v>1980.0</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M44" s="4"/>
       <c r="N44" s="6" t="s">
@@ -2210,7 +2210,7 @@
         <v>7118244</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
@@ -2297,10 +2297,10 @@
     </row>
     <row r="54" spans="1:14">
       <c r="A54" s="4">
-        <v>7143371</v>
+        <v>5787275</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -2315,7 +2315,7 @@
         <v>7</v>
       </c>
       <c r="K54" s="4">
-        <v>287.47</v>
+        <v>1010.6</v>
       </c>
       <c r="L54" s="5" t="s">
         <v>62</v>
@@ -2327,10 +2327,10 @@
     </row>
     <row r="55" spans="1:14">
       <c r="A55" s="4">
-        <v>5787275</v>
+        <v>7143371</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -2345,7 +2345,7 @@
         <v>7</v>
       </c>
       <c r="K55" s="4">
-        <v>1010.6</v>
+        <v>287.47</v>
       </c>
       <c r="L55" s="5" t="s">
         <v>62</v>
@@ -2597,10 +2597,10 @@
     </row>
     <row r="64" spans="1:14">
       <c r="A64" s="4">
-        <v>5787275</v>
+        <v>1899092</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -2615,10 +2615,10 @@
         <v>7</v>
       </c>
       <c r="K64" s="4">
-        <v>1010.6</v>
+        <v>770.0</v>
       </c>
       <c r="L64" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M64" s="4"/>
       <c r="N64" s="6" t="s">
@@ -2627,10 +2627,10 @@
     </row>
     <row r="65" spans="1:14">
       <c r="A65" s="4">
-        <v>1899092</v>
+        <v>5787275</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
@@ -2645,10 +2645,10 @@
         <v>7</v>
       </c>
       <c r="K65" s="4">
-        <v>770.0</v>
+        <v>1010.6</v>
       </c>
       <c r="L65" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M65" s="4"/>
       <c r="N65" s="6" t="s">
@@ -2990,7 +2990,7 @@
         <v>1899092</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -3167,10 +3167,10 @@
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="4">
-        <v>5684823</v>
+        <v>5787275</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -3185,7 +3185,7 @@
         <v>7</v>
       </c>
       <c r="K83" s="4">
-        <v>665.0</v>
+        <v>1010.6</v>
       </c>
       <c r="L83" s="5" t="s">
         <v>90</v>
@@ -3197,10 +3197,10 @@
     </row>
     <row r="84" spans="1:14">
       <c r="A84" s="4">
-        <v>5787275</v>
+        <v>5684823</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
@@ -3215,7 +3215,7 @@
         <v>7</v>
       </c>
       <c r="K84" s="4">
-        <v>1010.6</v>
+        <v>665.0</v>
       </c>
       <c r="L84" s="5" t="s">
         <v>90</v>
@@ -3227,10 +3227,10 @@
     </row>
     <row r="85" spans="1:14">
       <c r="A85" s="4">
-        <v>7259089</v>
+        <v>1899092</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
@@ -3245,7 +3245,7 @@
         <v>7</v>
       </c>
       <c r="K85" s="4">
-        <v>818.38</v>
+        <v>770.0</v>
       </c>
       <c r="L85" s="5" t="s">
         <v>91</v>
@@ -3257,10 +3257,10 @@
     </row>
     <row r="86" spans="1:14">
       <c r="A86" s="4">
-        <v>1899092</v>
+        <v>7259089</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
@@ -3275,7 +3275,7 @@
         <v>7</v>
       </c>
       <c r="K86" s="4">
-        <v>770.0</v>
+        <v>818.38</v>
       </c>
       <c r="L86" s="5" t="s">
         <v>91</v>
@@ -3377,10 +3377,10 @@
     </row>
     <row r="90" spans="1:14">
       <c r="A90" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
@@ -3395,7 +3395,7 @@
         <v>7</v>
       </c>
       <c r="K90" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L90" s="5" t="s">
         <v>95</v>
@@ -3407,10 +3407,10 @@
     </row>
     <row r="91" spans="1:14">
       <c r="A91" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
@@ -3425,7 +3425,7 @@
         <v>7</v>
       </c>
       <c r="K91" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L91" s="5" t="s">
         <v>95</v>
@@ -3467,10 +3467,10 @@
     </row>
     <row r="93" spans="1:14">
       <c r="A93" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
@@ -3485,7 +3485,7 @@
         <v>7</v>
       </c>
       <c r="K93" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L93" s="5" t="s">
         <v>97</v>
@@ -3497,10 +3497,10 @@
     </row>
     <row r="94" spans="1:14">
       <c r="A94" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
@@ -3515,7 +3515,7 @@
         <v>7</v>
       </c>
       <c r="K94" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L94" s="5" t="s">
         <v>97</v>
@@ -3527,10 +3527,10 @@
     </row>
     <row r="95" spans="1:14">
       <c r="A95" s="4">
-        <v>1899092</v>
+        <v>5684823</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
@@ -3545,7 +3545,7 @@
         <v>7</v>
       </c>
       <c r="K95" s="4">
-        <v>770.0</v>
+        <v>665.0</v>
       </c>
       <c r="L95" s="5" t="s">
         <v>98</v>
@@ -3557,10 +3557,10 @@
     </row>
     <row r="96" spans="1:14">
       <c r="A96" s="4">
-        <v>5684823</v>
+        <v>1899092</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
@@ -3575,7 +3575,7 @@
         <v>7</v>
       </c>
       <c r="K96" s="4">
-        <v>665.0</v>
+        <v>770.0</v>
       </c>
       <c r="L96" s="5" t="s">
         <v>98</v>
@@ -3737,10 +3737,10 @@
     </row>
     <row r="102" spans="1:14">
       <c r="A102" s="4">
-        <v>5684823</v>
+        <v>7259089</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -3755,7 +3755,7 @@
         <v>7</v>
       </c>
       <c r="K102" s="4">
-        <v>665.0</v>
+        <v>818.38</v>
       </c>
       <c r="L102" s="5" t="s">
         <v>103</v>
@@ -3797,10 +3797,10 @@
     </row>
     <row r="104" spans="1:14">
       <c r="A104" s="4">
-        <v>7259089</v>
+        <v>5684823</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
@@ -3815,7 +3815,7 @@
         <v>7</v>
       </c>
       <c r="K104" s="4">
-        <v>818.38</v>
+        <v>665.0</v>
       </c>
       <c r="L104" s="5" t="s">
         <v>103</v>
@@ -5356,7 +5356,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="73" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader>&amp;L2024-02-15 07:40:52&amp;C&amp;HECOMSOFT&amp;RDR. ORLANDO BEJARANO FERNANDEZ</oddHeader>
+    <oddHeader>&amp;L2024-02-16 06:34:08&amp;C&amp;HECOMSOFT&amp;RDR. ORLANDO BEJARANO FERNANDEZ</oddHeader>
     <oddFooter>&amp;RPage &amp;P of &amp;N</oddFooter>
     <evenHeader/>
     <evenFooter/>

</xml_diff>

<commit_message>
Cambios realizados el sabado 17-02 22:39
</commit_message>
<xml_diff>
--- a/public/week_data.xlsx
+++ b/public/week_data.xlsx
@@ -335,12 +335,12 @@
     <t>2022-12-05</t>
   </si>
   <si>
+    <t>JUANA ESTHER MICHEL CRUZ</t>
+  </si>
+  <si>
     <t>2022-12-12</t>
   </si>
   <si>
-    <t>JUANA ESTHER MICHEL CRUZ</t>
-  </si>
-  <si>
     <t>2022-12-13</t>
   </si>
   <si>
@@ -353,16 +353,16 @@
     <t>2022-12-21</t>
   </si>
   <si>
+    <t>LISELDA MILENIA ROMERO ALARCON</t>
+  </si>
+  <si>
+    <t>2022-12-22</t>
+  </si>
+  <si>
     <t>LIMBER RAYNARD GARNICA MEZZA</t>
   </si>
   <si>
-    <t>2022-12-22</t>
-  </si>
-  <si>
     <t>MARCO ANTONIO COLODRO</t>
-  </si>
-  <si>
-    <t>LISELDA MILENIA ROMERO ALARCON</t>
   </si>
   <si>
     <t>2022-12-26</t>
@@ -2657,10 +2657,10 @@
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="4">
-        <v>7143371</v>
+        <v>7254095</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -2675,7 +2675,7 @@
         <v>7</v>
       </c>
       <c r="K66" s="4">
-        <v>287.47</v>
+        <v>185.1</v>
       </c>
       <c r="L66" s="5" t="s">
         <v>76</v>
@@ -2687,10 +2687,10 @@
     </row>
     <row r="67" spans="1:14">
       <c r="A67" s="4">
-        <v>7254095</v>
+        <v>7143371</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -2705,7 +2705,7 @@
         <v>7</v>
       </c>
       <c r="K67" s="4">
-        <v>185.1</v>
+        <v>287.47</v>
       </c>
       <c r="L67" s="5" t="s">
         <v>76</v>
@@ -3077,10 +3077,10 @@
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -3095,7 +3095,7 @@
         <v>7</v>
       </c>
       <c r="K80" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L80" s="5" t="s">
         <v>88</v>
@@ -3107,10 +3107,10 @@
     </row>
     <row r="81" spans="1:14">
       <c r="A81" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -3125,7 +3125,7 @@
         <v>7</v>
       </c>
       <c r="K81" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L81" s="5" t="s">
         <v>88</v>
@@ -3167,10 +3167,10 @@
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="4">
-        <v>5787275</v>
+        <v>5684823</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -3185,7 +3185,7 @@
         <v>7</v>
       </c>
       <c r="K83" s="4">
-        <v>1010.6</v>
+        <v>665.0</v>
       </c>
       <c r="L83" s="5" t="s">
         <v>90</v>
@@ -3197,10 +3197,10 @@
     </row>
     <row r="84" spans="1:14">
       <c r="A84" s="4">
-        <v>5684823</v>
+        <v>5787275</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
@@ -3215,7 +3215,7 @@
         <v>7</v>
       </c>
       <c r="K84" s="4">
-        <v>665.0</v>
+        <v>1010.6</v>
       </c>
       <c r="L84" s="5" t="s">
         <v>90</v>
@@ -3647,10 +3647,10 @@
     </row>
     <row r="99" spans="1:14">
       <c r="A99" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -3665,7 +3665,7 @@
         <v>7</v>
       </c>
       <c r="K99" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L99" s="5" t="s">
         <v>101</v>
@@ -3677,10 +3677,10 @@
     </row>
     <row r="100" spans="1:14">
       <c r="A100" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -3695,7 +3695,7 @@
         <v>7</v>
       </c>
       <c r="K100" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L100" s="5" t="s">
         <v>101</v>
@@ -3917,10 +3917,10 @@
     </row>
     <row r="108" spans="1:14">
       <c r="A108" s="4">
-        <v>7254095</v>
+        <v>7103441</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
@@ -3935,10 +3935,10 @@
         <v>7</v>
       </c>
       <c r="K108" s="4">
-        <v>185.1</v>
+        <v>1480.0</v>
       </c>
       <c r="L108" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M108" s="4"/>
       <c r="N108" s="6" t="s">
@@ -3947,10 +3947,10 @@
     </row>
     <row r="109" spans="1:14">
       <c r="A109" s="4">
-        <v>7103441</v>
+        <v>7254095</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -3965,10 +3965,10 @@
         <v>7</v>
       </c>
       <c r="K109" s="4">
-        <v>1480.0</v>
+        <v>185.1</v>
       </c>
       <c r="L109" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M109" s="4"/>
       <c r="N109" s="6" t="s">
@@ -4067,7 +4067,7 @@
     </row>
     <row r="113" spans="1:14">
       <c r="A113" s="4">
-        <v>5797560</v>
+        <v>7247912</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>112</v>
@@ -4085,7 +4085,7 @@
         <v>7</v>
       </c>
       <c r="K113" s="4">
-        <v>320.0</v>
+        <v>8000.0</v>
       </c>
       <c r="L113" s="5" t="s">
         <v>113</v>
@@ -4097,7 +4097,7 @@
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="4">
-        <v>7190526</v>
+        <v>5797560</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>114</v>
@@ -4115,7 +4115,7 @@
         <v>7</v>
       </c>
       <c r="K114" s="4">
-        <v>57.0</v>
+        <v>320.0</v>
       </c>
       <c r="L114" s="5" t="s">
         <v>113</v>
@@ -4127,7 +4127,7 @@
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="4">
-        <v>7247912</v>
+        <v>7190526</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>115</v>
@@ -4145,7 +4145,7 @@
         <v>7</v>
       </c>
       <c r="K115" s="4">
-        <v>8000.0</v>
+        <v>57.0</v>
       </c>
       <c r="L115" s="5" t="s">
         <v>113</v>
@@ -4220,7 +4220,7 @@
         <v>7103441</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
@@ -4307,10 +4307,10 @@
     </row>
     <row r="121" spans="1:14">
       <c r="A121" s="4">
-        <v>7247912</v>
+        <v>5797560</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
@@ -4325,7 +4325,7 @@
         <v>7</v>
       </c>
       <c r="K121" s="4">
-        <v>8000.0</v>
+        <v>320.0</v>
       </c>
       <c r="L121" s="5" t="s">
         <v>121</v>
@@ -4337,10 +4337,10 @@
     </row>
     <row r="122" spans="1:14">
       <c r="A122" s="4">
-        <v>5797560</v>
+        <v>7190526</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
@@ -4355,7 +4355,7 @@
         <v>7</v>
       </c>
       <c r="K122" s="4">
-        <v>320.0</v>
+        <v>57.0</v>
       </c>
       <c r="L122" s="5" t="s">
         <v>121</v>
@@ -4367,10 +4367,10 @@
     </row>
     <row r="123" spans="1:14">
       <c r="A123" s="4">
-        <v>7190526</v>
+        <v>7247912</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
@@ -4385,7 +4385,7 @@
         <v>7</v>
       </c>
       <c r="K123" s="4">
-        <v>57.0</v>
+        <v>8000.0</v>
       </c>
       <c r="L123" s="5" t="s">
         <v>121</v>
@@ -4430,7 +4430,7 @@
         <v>7103441</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
@@ -4520,7 +4520,7 @@
         <v>5797560</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -4550,7 +4550,7 @@
         <v>7247912</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
@@ -4700,7 +4700,7 @@
         <v>7247912</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
@@ -4730,7 +4730,7 @@
         <v>5797560</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
@@ -5356,7 +5356,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="73" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader>&amp;L2024-02-16 06:34:08&amp;C&amp;HECOMSOFT&amp;RDR. ORLANDO BEJARANO FERNANDEZ</oddHeader>
+    <oddHeader>&amp;L2024-02-17 11:39:03&amp;C&amp;HECOMSOFT&amp;RDR. ORLANDO BEJARANO FERNANDEZ</oddHeader>
     <oddFooter>&amp;RPage &amp;P of &amp;N</oddFooter>
     <evenHeader/>
     <evenFooter/>

</xml_diff>

<commit_message>
Se modificó el encabezado del PDF para imprimir, de los clientes cobrables en pagos
</commit_message>
<xml_diff>
--- a/public/week_data.xlsx
+++ b/public/week_data.xlsx
@@ -335,12 +335,12 @@
     <t>2022-12-05</t>
   </si>
   <si>
+    <t>2022-12-12</t>
+  </si>
+  <si>
     <t>JUANA ESTHER MICHEL CRUZ</t>
   </si>
   <si>
-    <t>2022-12-12</t>
-  </si>
-  <si>
     <t>2022-12-13</t>
   </si>
   <si>
@@ -353,16 +353,16 @@
     <t>2022-12-21</t>
   </si>
   <si>
+    <t>LIMBER RAYNARD GARNICA MEZZA</t>
+  </si>
+  <si>
+    <t>2022-12-22</t>
+  </si>
+  <si>
+    <t>MARCO ANTONIO COLODRO</t>
+  </si>
+  <si>
     <t>LISELDA MILENIA ROMERO ALARCON</t>
-  </si>
-  <si>
-    <t>2022-12-22</t>
-  </si>
-  <si>
-    <t>LIMBER RAYNARD GARNICA MEZZA</t>
-  </si>
-  <si>
-    <t>MARCO ANTONIO COLODRO</t>
   </si>
   <si>
     <t>2022-12-26</t>
@@ -2297,10 +2297,10 @@
     </row>
     <row r="54" spans="1:14">
       <c r="A54" s="4">
-        <v>5787275</v>
+        <v>7143371</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -2315,7 +2315,7 @@
         <v>7</v>
       </c>
       <c r="K54" s="4">
-        <v>1010.6</v>
+        <v>287.47</v>
       </c>
       <c r="L54" s="5" t="s">
         <v>62</v>
@@ -2327,10 +2327,10 @@
     </row>
     <row r="55" spans="1:14">
       <c r="A55" s="4">
-        <v>7143371</v>
+        <v>5787275</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -2345,7 +2345,7 @@
         <v>7</v>
       </c>
       <c r="K55" s="4">
-        <v>287.47</v>
+        <v>1010.6</v>
       </c>
       <c r="L55" s="5" t="s">
         <v>62</v>
@@ -2657,10 +2657,10 @@
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="4">
-        <v>7254095</v>
+        <v>7143371</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -2675,7 +2675,7 @@
         <v>7</v>
       </c>
       <c r="K66" s="4">
-        <v>185.1</v>
+        <v>287.47</v>
       </c>
       <c r="L66" s="5" t="s">
         <v>76</v>
@@ -2687,10 +2687,10 @@
     </row>
     <row r="67" spans="1:14">
       <c r="A67" s="4">
-        <v>7143371</v>
+        <v>7254095</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -2705,7 +2705,7 @@
         <v>7</v>
       </c>
       <c r="K67" s="4">
-        <v>287.47</v>
+        <v>185.1</v>
       </c>
       <c r="L67" s="5" t="s">
         <v>76</v>
@@ -3077,10 +3077,10 @@
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -3095,7 +3095,7 @@
         <v>7</v>
       </c>
       <c r="K80" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L80" s="5" t="s">
         <v>88</v>
@@ -3107,10 +3107,10 @@
     </row>
     <row r="81" spans="1:14">
       <c r="A81" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -3125,7 +3125,7 @@
         <v>7</v>
       </c>
       <c r="K81" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L81" s="5" t="s">
         <v>88</v>
@@ -3167,10 +3167,10 @@
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="4">
-        <v>5684823</v>
+        <v>5787275</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -3185,7 +3185,7 @@
         <v>7</v>
       </c>
       <c r="K83" s="4">
-        <v>665.0</v>
+        <v>1010.6</v>
       </c>
       <c r="L83" s="5" t="s">
         <v>90</v>
@@ -3197,10 +3197,10 @@
     </row>
     <row r="84" spans="1:14">
       <c r="A84" s="4">
-        <v>5787275</v>
+        <v>5684823</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
@@ -3215,7 +3215,7 @@
         <v>7</v>
       </c>
       <c r="K84" s="4">
-        <v>1010.6</v>
+        <v>665.0</v>
       </c>
       <c r="L84" s="5" t="s">
         <v>90</v>
@@ -3647,10 +3647,10 @@
     </row>
     <row r="99" spans="1:14">
       <c r="A99" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -3665,7 +3665,7 @@
         <v>7</v>
       </c>
       <c r="K99" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L99" s="5" t="s">
         <v>101</v>
@@ -3677,10 +3677,10 @@
     </row>
     <row r="100" spans="1:14">
       <c r="A100" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -3695,7 +3695,7 @@
         <v>7</v>
       </c>
       <c r="K100" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L100" s="5" t="s">
         <v>101</v>
@@ -3737,10 +3737,10 @@
     </row>
     <row r="102" spans="1:14">
       <c r="A102" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -3755,7 +3755,7 @@
         <v>7</v>
       </c>
       <c r="K102" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L102" s="5" t="s">
         <v>103</v>
@@ -3767,10 +3767,10 @@
     </row>
     <row r="103" spans="1:14">
       <c r="A103" s="4">
-        <v>7254095</v>
+        <v>5684823</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
@@ -3785,7 +3785,7 @@
         <v>7</v>
       </c>
       <c r="K103" s="4">
-        <v>185.1</v>
+        <v>665.0</v>
       </c>
       <c r="L103" s="5" t="s">
         <v>103</v>
@@ -3797,10 +3797,10 @@
     </row>
     <row r="104" spans="1:14">
       <c r="A104" s="4">
-        <v>5684823</v>
+        <v>7259089</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
@@ -3815,7 +3815,7 @@
         <v>7</v>
       </c>
       <c r="K104" s="4">
-        <v>665.0</v>
+        <v>818.38</v>
       </c>
       <c r="L104" s="5" t="s">
         <v>103</v>
@@ -3917,10 +3917,10 @@
     </row>
     <row r="108" spans="1:14">
       <c r="A108" s="4">
-        <v>7103441</v>
+        <v>7254095</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
@@ -3935,10 +3935,10 @@
         <v>7</v>
       </c>
       <c r="K108" s="4">
-        <v>1480.0</v>
+        <v>185.1</v>
       </c>
       <c r="L108" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M108" s="4"/>
       <c r="N108" s="6" t="s">
@@ -3947,10 +3947,10 @@
     </row>
     <row r="109" spans="1:14">
       <c r="A109" s="4">
-        <v>7254095</v>
+        <v>7103441</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -3965,10 +3965,10 @@
         <v>7</v>
       </c>
       <c r="K109" s="4">
-        <v>185.1</v>
+        <v>1480.0</v>
       </c>
       <c r="L109" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M109" s="4"/>
       <c r="N109" s="6" t="s">
@@ -4067,7 +4067,7 @@
     </row>
     <row r="113" spans="1:14">
       <c r="A113" s="4">
-        <v>7247912</v>
+        <v>5797560</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>112</v>
@@ -4085,7 +4085,7 @@
         <v>7</v>
       </c>
       <c r="K113" s="4">
-        <v>8000.0</v>
+        <v>320.0</v>
       </c>
       <c r="L113" s="5" t="s">
         <v>113</v>
@@ -4097,7 +4097,7 @@
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="4">
-        <v>5797560</v>
+        <v>7190526</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>114</v>
@@ -4115,7 +4115,7 @@
         <v>7</v>
       </c>
       <c r="K114" s="4">
-        <v>320.0</v>
+        <v>57.0</v>
       </c>
       <c r="L114" s="5" t="s">
         <v>113</v>
@@ -4127,7 +4127,7 @@
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="4">
-        <v>7190526</v>
+        <v>7247912</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>115</v>
@@ -4145,7 +4145,7 @@
         <v>7</v>
       </c>
       <c r="K115" s="4">
-        <v>57.0</v>
+        <v>8000.0</v>
       </c>
       <c r="L115" s="5" t="s">
         <v>113</v>
@@ -4220,7 +4220,7 @@
         <v>7103441</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
@@ -4307,10 +4307,10 @@
     </row>
     <row r="121" spans="1:14">
       <c r="A121" s="4">
-        <v>5797560</v>
+        <v>7247912</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
@@ -4325,7 +4325,7 @@
         <v>7</v>
       </c>
       <c r="K121" s="4">
-        <v>320.0</v>
+        <v>8000.0</v>
       </c>
       <c r="L121" s="5" t="s">
         <v>121</v>
@@ -4337,10 +4337,10 @@
     </row>
     <row r="122" spans="1:14">
       <c r="A122" s="4">
-        <v>7190526</v>
+        <v>5797560</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
@@ -4355,7 +4355,7 @@
         <v>7</v>
       </c>
       <c r="K122" s="4">
-        <v>57.0</v>
+        <v>320.0</v>
       </c>
       <c r="L122" s="5" t="s">
         <v>121</v>
@@ -4367,10 +4367,10 @@
     </row>
     <row r="123" spans="1:14">
       <c r="A123" s="4">
-        <v>7247912</v>
+        <v>7190526</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
@@ -4385,7 +4385,7 @@
         <v>7</v>
       </c>
       <c r="K123" s="4">
-        <v>8000.0</v>
+        <v>57.0</v>
       </c>
       <c r="L123" s="5" t="s">
         <v>121</v>
@@ -4430,7 +4430,7 @@
         <v>7103441</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
@@ -4520,7 +4520,7 @@
         <v>5797560</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -4550,7 +4550,7 @@
         <v>7247912</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
@@ -4700,7 +4700,7 @@
         <v>7247912</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
@@ -4730,7 +4730,7 @@
         <v>5797560</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
@@ -5356,7 +5356,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="73" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader>&amp;L2024-02-17 11:39:03&amp;C&amp;HECOMSOFT&amp;RDR. ORLANDO BEJARANO FERNANDEZ</oddHeader>
+    <oddHeader>&amp;L2024-02-18 01:54:35&amp;C&amp;HECOMSOFT&amp;RDR. ORLANDO BEJARANO FERNANDEZ</oddHeader>
     <oddFooter>&amp;RPage &amp;P of &amp;N</oddFooter>
     <evenHeader/>
     <evenFooter/>

</xml_diff>